<commit_message>
Acrescenta a coluna de diabéticos preenchida com interpolação
Acrescenta a coluna de diabéticos preenchida com interpolação e altera o nome das colunas
</commit_message>
<xml_diff>
--- a/datateste_diabetes1.2.xlsx
+++ b/datateste_diabetes1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah220043\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{807F1C20-37DA-4D22-9C1A-FED1398467D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA83D421-9876-458A-AF73-9899FB7B5E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="510" windowWidth="15930" windowHeight="9440" xr2:uid="{C79C5FAE-2211-40DA-8695-D333B7B81CC2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C79C5FAE-2211-40DA-8695-D333B7B81CC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,25 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="96">
-  <si>
-    <t>Ano</t>
-  </si>
-  <si>
-    <t>País</t>
-  </si>
-  <si>
-    <t>IDH</t>
-  </si>
-  <si>
-    <t>População</t>
-  </si>
-  <si>
-    <t>Porcentagem de crianças abaixo de 5 anos que estão com soprepeso(FAO)</t>
-  </si>
-  <si>
-    <t>Necessidade média de energia da dieta (kcal/cap/day) FAO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="150">
   <si>
     <t>Brasil</t>
   </si>
@@ -323,6 +305,186 @@
   </si>
   <si>
     <t>0.767</t>
+  </si>
+  <si>
+    <t>15733.6</t>
+  </si>
+  <si>
+    <t>3310. 4</t>
+  </si>
+  <si>
+    <t>1806.8</t>
+  </si>
+  <si>
+    <t>1531.8</t>
+  </si>
+  <si>
+    <t>760.9</t>
+  </si>
+  <si>
+    <t>1747.1</t>
+  </si>
+  <si>
+    <t>1190.1</t>
+  </si>
+  <si>
+    <t>131.1</t>
+  </si>
+  <si>
+    <t>246.69</t>
+  </si>
+  <si>
+    <t>358.42</t>
+  </si>
+  <si>
+    <t>466.29</t>
+  </si>
+  <si>
+    <t>570.29</t>
+  </si>
+  <si>
+    <t>670.42</t>
+  </si>
+  <si>
+    <t>766.70</t>
+  </si>
+  <si>
+    <t>859.11</t>
+  </si>
+  <si>
+    <t>947.65</t>
+  </si>
+  <si>
+    <t>1032.3</t>
+  </si>
+  <si>
+    <t>1113.1</t>
+  </si>
+  <si>
+    <t>1263.2</t>
+  </si>
+  <si>
+    <t>1332.4</t>
+  </si>
+  <si>
+    <t>1397.8</t>
+  </si>
+  <si>
+    <t>1459.3</t>
+  </si>
+  <si>
+    <t>1516.9</t>
+  </si>
+  <si>
+    <t>1570.7</t>
+  </si>
+  <si>
+    <t>1620.6</t>
+  </si>
+  <si>
+    <t>1666.6</t>
+  </si>
+  <si>
+    <t>1708.8</t>
+  </si>
+  <si>
+    <t>851.26</t>
+  </si>
+  <si>
+    <t>937.56</t>
+  </si>
+  <si>
+    <t>1019.8</t>
+  </si>
+  <si>
+    <t>1098.0</t>
+  </si>
+  <si>
+    <t>1172.1</t>
+  </si>
+  <si>
+    <t>1242.2</t>
+  </si>
+  <si>
+    <t>1308.2</t>
+  </si>
+  <si>
+    <t>1370.2</t>
+  </si>
+  <si>
+    <t>1428.1</t>
+  </si>
+  <si>
+    <t>1482.0</t>
+  </si>
+  <si>
+    <t>1577.5</t>
+  </si>
+  <si>
+    <t>1619.2</t>
+  </si>
+  <si>
+    <t>1656.9</t>
+  </si>
+  <si>
+    <t>1690.5</t>
+  </si>
+  <si>
+    <t>1720.0</t>
+  </si>
+  <si>
+    <t>1745.5</t>
+  </si>
+  <si>
+    <t>1766.9</t>
+  </si>
+  <si>
+    <t>1784.2</t>
+  </si>
+  <si>
+    <t>1797.5</t>
+  </si>
+  <si>
+    <t>4378.7</t>
+  </si>
+  <si>
+    <t>3299.4</t>
+  </si>
+  <si>
+    <t>6372.4</t>
+  </si>
+  <si>
+    <t>7297.7</t>
+  </si>
+  <si>
+    <t>8175.4</t>
+  </si>
+  <si>
+    <t>9005.3</t>
+  </si>
+  <si>
+    <t>9787.6</t>
+  </si>
+  <si>
+    <t>ano</t>
+  </si>
+  <si>
+    <t>pais</t>
+  </si>
+  <si>
+    <t>idh</t>
+  </si>
+  <si>
+    <t>populacao_geral</t>
+  </si>
+  <si>
+    <t>per_crian_cinc_soprep</t>
+  </si>
+  <si>
+    <t>kcal_medio</t>
+  </si>
+  <si>
+    <t>diabeticos</t>
   </si>
 </sst>
 </file>
@@ -777,44 +939,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622E5C0E-D197-4525-9BDB-A803C3516223}">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="16.81640625" customWidth="1"/>
-    <col min="5" max="5" width="9.36328125" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
+    <col min="6" max="6" width="27.08984375" customWidth="1"/>
+    <col min="8" max="8" width="21.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>145</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>146</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>147</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>148</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>2021</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="4">
@@ -824,141 +991,162 @@
       <c r="F2" s="6">
         <v>2447</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H2" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7">
         <f>SUM(A2-1)</f>
         <v>2020</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="4">
         <v>212559409</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F3" s="5">
         <v>2448</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H3" s="1">
+        <v>15619</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7">
         <f>SUM(A3-1)</f>
         <v>2019</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D4" s="4">
         <v>211049519</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F4" s="5">
         <v>2447</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H4" s="1">
+        <v>15456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7">
         <f t="shared" ref="A5:A23" si="0">SUM(A4-1)</f>
         <v>2018</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D5" s="4">
         <v>209469320</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F5" s="5">
         <v>2447</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H5" s="1">
+        <v>15246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7">
         <f t="shared" si="0"/>
         <v>2017</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D6" s="4">
         <v>207833825</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F6" s="5">
         <v>2446</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H6" s="1">
+        <v>14988</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="7">
         <f t="shared" si="0"/>
         <v>2016</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D7" s="4">
         <v>206163056</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F7" s="5">
         <v>2446</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H7" s="1">
+        <v>14683</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="7">
         <f t="shared" si="0"/>
         <v>2015</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D8" s="4">
         <v>204471759</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F8" s="5">
         <v>2445</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H8" s="1">
+        <v>14330</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7">
         <f t="shared" si="0"/>
         <v>2014</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D9" s="4">
         <v>202763744</v>
@@ -969,307 +1157,352 @@
       <c r="F9" s="5">
         <v>2443</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H9" s="1">
+        <v>13929</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="7">
         <f t="shared" si="0"/>
         <v>2013</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D10" s="4">
         <v>201035904</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F10" s="5">
         <v>2442</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H10" s="1">
+        <v>13480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="7">
         <f t="shared" si="0"/>
         <v>2012</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D11" s="4">
         <v>199287292</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F11" s="5">
         <v>2439</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H11" s="1">
+        <v>12984</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="7">
         <f t="shared" si="0"/>
         <v>2011</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D12" s="4">
         <v>197514541</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F12" s="5">
         <v>2436</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H12" s="1">
+        <v>12440</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="7">
         <f t="shared" si="0"/>
         <v>2010</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D13" s="4">
         <v>195713637</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F13" s="5">
         <v>2433</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H13" s="1">
+        <v>11848</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="7">
         <f t="shared" si="0"/>
         <v>2009</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D14" s="4">
         <v>193886505</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F14" s="5">
         <v>2429</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H14" s="1">
+        <v>11209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="7">
         <f t="shared" si="0"/>
         <v>2008</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D15" s="4">
-        <v>192030362</v>
+        <v>10522</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F15" s="5">
         <v>2424</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H15" s="1">
+        <v>10522</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="7">
         <f t="shared" si="0"/>
         <v>2007</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D16" s="4">
         <v>190130445</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F16" s="5">
         <v>2417</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H16" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="7">
         <f t="shared" si="0"/>
         <v>2006</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D17" s="4">
         <v>188167353</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F17" s="5">
         <v>2409</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H17" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="7">
         <f t="shared" si="0"/>
         <v>2005</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D18" s="4">
         <v>186127108</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F18" s="5">
         <v>2401</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H18" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="7">
         <f t="shared" si="0"/>
         <v>2004</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D19" s="4">
         <v>184006479</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F19" s="5">
         <v>2393</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H19" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="7">
         <f t="shared" si="0"/>
         <v>2003</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D20" s="4">
         <v>181809244</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F20" s="5">
         <v>2385</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H20" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="7">
         <f t="shared" si="0"/>
         <v>2002</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D21" s="4">
         <v>179537523</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F21" s="5">
         <v>2376</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H21" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="7">
         <f t="shared" si="0"/>
         <v>2001</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D22" s="4">
         <v>177196051</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F22" s="5">
         <v>2371</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H22" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="7">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D23" s="4">
         <v>174790339</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F23" s="8">
         <v>2367</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H23" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>2021</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="4">
@@ -1279,351 +1512,402 @@
       <c r="F24" s="5">
         <v>2417</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H24" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="7">
         <f>SUM(A24-1)</f>
         <v>2020</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="4">
         <v>45376763</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F25" s="5">
         <v>2416</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H25" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="7">
         <f t="shared" ref="A26:A45" si="1">SUM(A25-1)</f>
         <v>2019</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D26" s="4">
         <v>44938712</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F26" s="5">
         <v>2414</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H26" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="7">
         <f t="shared" si="1"/>
         <v>2018</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D27" s="4">
         <v>44494502</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F27" s="5">
         <v>2412</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H27" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="7">
         <f t="shared" si="1"/>
         <v>2017</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D28" s="4">
         <v>44044811</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F28" s="5">
         <v>2412</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H28" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="7">
         <f t="shared" si="1"/>
         <v>2016</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D29" s="4">
         <v>43590368</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F29" s="5">
         <v>2411</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H29" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="7">
         <f t="shared" si="1"/>
         <v>2015</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D30" s="4">
         <v>43131966</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F30" s="5">
         <v>2410</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H30" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="7">
         <f t="shared" si="1"/>
         <v>2014</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D31" s="4">
         <v>42669500</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F31" s="5">
         <v>2409</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H31" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="7">
         <f t="shared" si="1"/>
         <v>2013</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D32" s="4">
         <v>42202935</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F32" s="5">
         <v>2408</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H32" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="7">
         <f t="shared" si="1"/>
         <v>2012</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D33" s="4">
         <v>41733271</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F33" s="5">
         <v>2407</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H33" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="7">
         <f t="shared" si="1"/>
         <v>2011</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D34" s="4">
         <v>41261490</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F34" s="5">
         <v>2406</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H34" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="7">
         <f t="shared" si="1"/>
         <v>2010</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D35" s="4">
         <v>40788453</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F35" s="5">
         <v>2405</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H35" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="7">
         <f t="shared" si="1"/>
         <v>2009</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D36" s="4">
         <v>40482786</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F36" s="5">
         <v>2403</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H36" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="7">
         <f t="shared" si="1"/>
         <v>2008</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D37" s="4">
         <v>40080159</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F37" s="5">
         <v>2401</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H37" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="7">
         <f t="shared" si="1"/>
         <v>2007</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D38" s="4">
         <v>39684303</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F38" s="5">
         <v>2398</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H38" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="7">
         <f t="shared" si="1"/>
         <v>2006</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D39" s="4">
         <v>39289876</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F39" s="5">
         <v>2396</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H39" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="7">
         <f t="shared" si="1"/>
         <v>2005</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D40" s="4">
         <v>38892924</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F40" s="5">
         <v>2395</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H40" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="7">
         <f t="shared" si="1"/>
         <v>2004</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D41" s="4">
         <v>38491970</v>
@@ -1634,97 +1918,112 @@
       <c r="F41" s="5">
         <v>2392</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H41" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="7">
         <f t="shared" si="1"/>
         <v>2003</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D42" s="4">
         <v>38087866</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F42" s="5">
         <v>2390</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H42" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="7">
         <f t="shared" si="1"/>
         <v>2002</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D43" s="4">
         <v>37681743</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F43" s="5">
         <v>2388</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H43" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="7">
         <f t="shared" si="1"/>
         <v>2001</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D44" s="4">
         <v>37275644</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F44" s="8">
         <v>2385</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H44" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="7">
         <f t="shared" si="1"/>
         <v>2000</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D45" s="4">
         <v>36870796</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F45" s="9">
         <v>2381</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H45" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="7">
         <v>2021</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="4">
@@ -1734,78 +2033,90 @@
       <c r="F46" s="10">
         <v>2443</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H46" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="7">
         <f>SUM(A46-1)</f>
         <v>2020</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="4">
         <v>19116209</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F47" s="10">
         <v>2442</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H47" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="7">
         <f t="shared" ref="A48:A67" si="2">SUM(A47-1)</f>
         <v>2019</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D48" s="4">
         <v>18952035</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F48" s="10">
         <v>2440</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H48" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="7">
         <f t="shared" si="2"/>
         <v>2018</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D49" s="4">
         <v>18729166</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F49" s="10">
         <v>2438</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H49" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="7">
         <f t="shared" si="2"/>
         <v>2017</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D50" s="4">
         <v>18470435</v>
@@ -1816,17 +2127,20 @@
       <c r="F50" s="10">
         <v>2435</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H50" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="7">
         <f t="shared" si="2"/>
         <v>2016</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D51" s="4">
         <v>18209072</v>
@@ -1837,341 +2151,392 @@
       <c r="F51" s="10">
         <v>2433</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H51" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="7">
         <f t="shared" si="2"/>
         <v>2015</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D52" s="4">
         <v>17969356</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F52" s="10">
         <v>2431</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H52" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="7">
         <f t="shared" si="2"/>
         <v>2014</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D53" s="4">
         <v>17758969</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F53" s="10">
         <v>2430</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H53" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="7">
         <f t="shared" si="2"/>
         <v>2013</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D54" s="4">
         <v>17571511</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F54" s="10">
         <v>2429</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H54" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="7">
         <f t="shared" si="2"/>
         <v>2012</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D55" s="4">
         <v>17400359</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F55" s="10">
         <v>2429</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H55" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="7">
         <f t="shared" si="2"/>
         <v>2011</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D56" s="4">
         <v>17233584</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F56" s="10">
         <v>2428</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H56" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="7">
         <f t="shared" si="2"/>
         <v>2010</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D57" s="4">
         <v>17062531</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F57" s="10">
         <v>2427</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H57" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="7">
         <f t="shared" si="2"/>
         <v>2009</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D58" s="4">
         <v>16886184</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F58" s="10">
         <v>2424</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H58" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="7">
         <f t="shared" si="2"/>
         <v>2008</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D59" s="4">
         <v>16708255</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F59" s="10">
         <v>2421</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H59" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="7">
         <f t="shared" si="2"/>
         <v>2007</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D60" s="4">
         <v>16530201</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F60" s="10">
         <v>2418</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H60" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="7">
         <f t="shared" si="2"/>
         <v>2006</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D61" s="4">
         <v>16354507</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F61" s="10">
         <v>2414</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H61" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="7">
         <f t="shared" si="2"/>
         <v>2005</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D62" s="4">
         <v>16182713</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F62" s="10">
         <v>2409</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H62" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="7">
         <f t="shared" si="2"/>
         <v>2004</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D63" s="4">
         <v>16014972</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F63" s="10">
         <v>2403</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H63" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="7">
         <f t="shared" si="2"/>
         <v>2003</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D64" s="4">
         <v>15849649</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F64" s="10">
         <v>2397</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H64" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="7">
         <f t="shared" si="2"/>
         <v>2002</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D65" s="4">
         <v>15684413</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F65" s="10">
         <v>2391</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H65" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="7">
         <f t="shared" si="2"/>
         <v>2001</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D66" s="4">
         <v>15516112</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F66" s="10">
         <v>2386</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H66" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="7">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D67" s="4">
         <v>15342350</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F67" s="10">
         <v>2378</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>